<commit_message>
completed Present teaching story
</commit_message>
<xml_diff>
--- a/assets/story/past.xlsx
+++ b/assets/story/past.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\OneDrive\เอกสาร\GitHub\testgame\assets\story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01CD6A7-7FDB-40F0-AEB3-4E5FF2D7CD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FC7C84-4F23-49CD-97A4-99F58CE57828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3772592E-09F7-4FC1-92FB-E4DBE6D3531A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>name</t>
   </si>
@@ -104,9 +104,6 @@
     <t>"You used to be an enthusiastic police officer."</t>
   </si>
   <si>
-    <t>ก็บอกว่าไม่ได้ว่าใครไงเล่า!?</t>
-  </si>
-  <si>
     <t>ไป ๆ ไปตรวจตราได้แล้ว!</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>โถ่ หัวหน้า...</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>ไม่ต้องมาทำหน้าสงสารเลยโว้ย!</t>
   </si>
   <si>
@@ -327,6 +321,21 @@
   </si>
   <si>
     <t>คุณเก่งมากที่เรียนรู้มาอยู่จุดนี้ได้ ตั้งใจทำงานล่ะ!</t>
+  </si>
+  <si>
+    <t>เอ๋!?</t>
+  </si>
+  <si>
+    <t>ก็บอกว่าไม่ได้ว่าใครไง!?</t>
+  </si>
+  <si>
+    <t>เฮ้อ อีกอย่างหนึ่งนะ ถ้าเป็นคำถามก็ใช้ did มาช่วย</t>
+  </si>
+  <si>
+    <t>พอเป็นมี did แล้ว verb ตัวอื่นจะต้องกลายเป็น V1</t>
+  </si>
+  <si>
+    <t>ที่ผมจะบอกก็มีเท่านี้แหละ</t>
   </si>
 </sst>
 </file>
@@ -716,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B8DC8F-8F8D-4240-96BA-843CD2C2EADB}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="87" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -731,16 +740,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -754,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -762,14 +771,14 @@
     </row>
     <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <f t="shared" ref="A3:A24" si="0">A2</f>
+        <f t="shared" ref="A3:A27" si="0">A2</f>
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f t="shared" ref="C3:C24" si="1">C2</f>
+        <f t="shared" ref="C3:C22" si="1">C2</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -992,11 +1001,8 @@
       <c r="B17" s="3">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1079,7 +1085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1087,12 +1093,8 @@
       <c r="B23" s="3">
         <v>22</v>
       </c>
-      <c r="C23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Grammar police chief</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1103,106 +1105,105 @@
       <c r="B24" s="3">
         <v>23</v>
       </c>
-      <c r="C24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Grammar police chief</v>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>C24</f>
+        <v>Grammar police chief</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B26" s="3">
         <v>25</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <f t="shared" ref="A26:A51" si="2">A25</f>
-        <v>2</v>
-      </c>
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
       <c r="C26" s="1" t="str">
-        <f t="shared" ref="C26:C45" si="3">C25</f>
+        <f>C25</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B27" s="3">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f>C26</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>A24</f>
+        <v>1</v>
       </c>
       <c r="B28" s="3">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f>C24</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B29" s="3">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Grammar police chief</v>
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A30:A55" si="2">A29</f>
         <v>2</v>
       </c>
       <c r="B30" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C30" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C30:C49" si="3">C29</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1211,14 +1212,14 @@
         <v>2</v>
       </c>
       <c r="B31" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C31" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1227,14 +1228,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C32" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1243,14 +1244,14 @@
         <v>2</v>
       </c>
       <c r="B33" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C33" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1259,14 +1260,14 @@
         <v>2</v>
       </c>
       <c r="B34" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1275,14 +1276,14 @@
         <v>2</v>
       </c>
       <c r="B35" s="3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1291,14 +1292,14 @@
         <v>2</v>
       </c>
       <c r="B36" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C36" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1307,14 +1308,14 @@
         <v>2</v>
       </c>
       <c r="B37" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1323,46 +1324,46 @@
         <v>2</v>
       </c>
       <c r="B38" s="3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B39" s="3">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B40" s="3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1371,14 +1372,14 @@
         <v>2</v>
       </c>
       <c r="B41" s="3">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1387,74 +1388,78 @@
         <v>2</v>
       </c>
       <c r="B42" s="3">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B43" s="3">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="70" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B44" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B45" s="3">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B46" s="3">
+        <v>18</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Grammar police chief</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="3">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B46" s="3">
-        <v>22</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1463,61 +1468,58 @@
         <v>2</v>
       </c>
       <c r="B47" s="3">
-        <v>23</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Grammar police chief</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="70" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B48" s="3">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C48" s="1" t="str">
-        <f t="shared" ref="C48:C51" si="4">C47</f>
+        <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B49" s="3">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C49" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B50" s="3">
-        <v>26</v>
-      </c>
-      <c r="C50" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Grammar police chief</v>
+        <v>22</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1526,124 +1528,123 @@
         <v>2</v>
       </c>
       <c r="B51" s="3">
-        <v>27</v>
-      </c>
-      <c r="C51" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Grammar police chief</v>
+        <v>23</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B52" s="3">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <f t="shared" ref="C52:C55" si="4">C51</f>
+        <v>Grammar police chief</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <f t="shared" ref="A53:A66" si="5">A52</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B53" s="3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1" t="str">
-        <f t="shared" ref="C53:C66" si="6">C52</f>
+        <f t="shared" si="4"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B54" s="3">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C54" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B55" s="3">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C55" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B56" s="3">
-        <v>5</v>
-      </c>
-      <c r="C56" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Grammar police chief</v>
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="A57:A70" si="5">A56</f>
         <v>3</v>
       </c>
       <c r="B57" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C57" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="C57:C70" si="6">C56</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B58" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C58" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1652,14 +1653,14 @@
         <v>3</v>
       </c>
       <c r="B59" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1668,14 +1669,14 @@
         <v>3</v>
       </c>
       <c r="B60" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C60" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1684,62 +1685,62 @@
         <v>3</v>
       </c>
       <c r="B61" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C61" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B62" s="3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B63" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B64" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C64" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1748,135 +1749,136 @@
         <v>3</v>
       </c>
       <c r="B65" s="3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C65" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B66" s="3">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C66" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="B67" s="3">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="C67" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Grammar police chief</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
-        <f t="shared" ref="A68:A91" si="7">A67</f>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="B68" s="3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C68" s="1" t="str">
-        <f>C67</f>
+        <f t="shared" si="6"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="B69" s="3">
+        <v>14</v>
+      </c>
+      <c r="C69" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Grammar police chief</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="A70" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
       <c r="B70" s="3">
-        <v>4</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="C70" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Grammar police chief</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B71" s="3">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1" t="str">
-        <f t="shared" ref="C71:C75" si="8">C70</f>
-        <v>Grammar police chief</v>
+        <v>1</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A72:A95" si="7">A71</f>
         <v>4</v>
       </c>
       <c r="B72" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C72" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>C71</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B73" s="3">
-        <v>7</v>
-      </c>
-      <c r="C73" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Grammar police chief</v>
+        <v>3</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1885,14 +1887,13 @@
         <v>4</v>
       </c>
       <c r="B74" s="3">
-        <v>8</v>
-      </c>
-      <c r="C74" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>Grammar police chief</v>
+        <v>4</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1901,26 +1902,30 @@
         <v>4</v>
       </c>
       <c r="B75" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="C75:C79" si="8">C74</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B76" s="3">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C76" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Grammar police chief</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1929,13 +1934,14 @@
         <v>4</v>
       </c>
       <c r="B77" s="3">
-        <v>11</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="C77" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Grammar police chief</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1944,14 +1950,14 @@
         <v>4</v>
       </c>
       <c r="B78" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C78" s="1" t="str">
-        <f t="shared" ref="C78:C88" si="9">C77</f>
+        <f t="shared" si="8"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1960,30 +1966,26 @@
         <v>4</v>
       </c>
       <c r="B79" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C79" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B80" s="3">
-        <v>14</v>
-      </c>
-      <c r="C80" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Grammar police chief</v>
+        <v>10</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -1992,30 +1994,29 @@
         <v>4</v>
       </c>
       <c r="B81" s="3">
-        <v>15</v>
-      </c>
-      <c r="C81" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>Grammar police chief</v>
+        <v>11</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="47.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B82" s="3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C82" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="C82:C92" si="9">C81</f>
         <v>Grammar police chief</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -2024,30 +2025,30 @@
         <v>4</v>
       </c>
       <c r="B83" s="3">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C83" s="1" t="str">
         <f t="shared" si="9"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="56" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B84" s="3">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C84" s="1" t="str">
         <f t="shared" si="9"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -2056,30 +2057,30 @@
         <v>4</v>
       </c>
       <c r="B85" s="3">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C85" s="1" t="str">
         <f t="shared" si="9"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="47.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B86" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C86" s="1" t="str">
         <f t="shared" si="9"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -2088,57 +2089,62 @@
         <v>4</v>
       </c>
       <c r="B87" s="3">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C87" s="1" t="str">
         <f t="shared" si="9"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="56" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B88" s="3">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C88" s="1" t="str">
         <f t="shared" si="9"/>
         <v>Grammar police chief</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B89" s="3">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="C89" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Grammar police chief</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B90" s="3">
-        <v>24</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C90" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Grammar police chief</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="28" x14ac:dyDescent="0.3">
@@ -2147,14 +2153,73 @@
         <v>4</v>
       </c>
       <c r="B91" s="3">
+        <v>21</v>
+      </c>
+      <c r="C91" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Grammar police chief</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B92" s="3">
+        <v>22</v>
+      </c>
+      <c r="C92" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Grammar police chief</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B93" s="3">
+        <v>23</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B94" s="3">
+        <v>24</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B95" s="3">
         <v>25</v>
       </c>
-      <c r="C91" s="1" t="str">
-        <f>C90</f>
-        <v>Grammar police chief</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>96</v>
+      <c r="C95" s="1" t="str">
+        <f>C94</f>
+        <v>Grammar police chief</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>